<commit_message>
Update models and YAMLs
</commit_message>
<xml_diff>
--- a/BC Curation Template.xlsx
+++ b/BC Curation Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda\Documents\CDISC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DD2F81-7F34-49EB-8862-F021A39FD60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE51D823-3938-48AA-B169-F59A63D71702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="3" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Conceptual VS BC" sheetId="6" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13267" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13283" uniqueCount="1280">
   <si>
     <t>C164634</t>
   </si>
@@ -3928,6 +3928,12 @@
   </si>
   <si>
     <t>3-87</t>
+  </si>
+  <si>
+    <t>sdtmig_end_version</t>
+  </si>
+  <si>
+    <t>An ordinal measurement of glucose present in a sample (placeholder)</t>
   </si>
 </sst>
 </file>
@@ -4148,7 +4154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4354,12 +4360,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4677,14 +4686,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B92937E-F1B4-4F44-9F47-44A7FBEED699}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="90" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.64453125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.234375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.9375" style="2" bestFit="1" customWidth="1"/>
@@ -4702,26 +4711,26 @@
     <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="92" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:15" s="91" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A1" s="90" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="91" t="s">
         <v>1034</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="91" t="s">
         <v>788</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="91" t="s">
         <v>789</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="91" t="s">
         <v>790</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="91" t="s">
         <v>1101</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="91" t="s">
         <v>796</v>
       </c>
       <c r="H1" s="10" t="s">
@@ -4733,16 +4742,16 @@
       <c r="J1" s="10" t="s">
         <v>875</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="91" t="s">
         <v>876</v>
       </c>
-      <c r="L1" s="92" t="s">
+      <c r="L1" s="91" t="s">
         <v>792</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="91" t="s">
         <v>793</v>
       </c>
-      <c r="N1" s="92" t="s">
+      <c r="N1" s="91" t="s">
         <v>794</v>
       </c>
       <c r="O1" s="10" t="s">
@@ -4750,7 +4759,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4791,7 +4800,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4817,7 +4826,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4846,7 +4855,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4879,7 +4888,7 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4908,7 +4917,7 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -4934,7 +4943,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4954,7 +4963,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="86" x14ac:dyDescent="0.3">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4998,7 +5007,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="9" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -5043,7 +5052,7 @@
       <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -5073,7 +5082,7 @@
       <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -5105,7 +5114,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -5137,7 +5146,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -5169,7 +5178,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="9" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -5201,7 +5210,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="9" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -5235,7 +5244,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="9" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5280,7 +5289,7 @@
       <c r="O17" s="16"/>
     </row>
     <row r="18" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -5310,7 +5319,7 @@
       <c r="O18" s="16"/>
     </row>
     <row r="19" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -5342,7 +5351,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -5374,7 +5383,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -5406,7 +5415,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="9" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -5438,7 +5447,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="9" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -5470,7 +5479,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="43" x14ac:dyDescent="0.5">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5496,7 +5505,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5522,7 +5531,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -5551,7 +5560,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5580,7 +5589,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -5609,7 +5618,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -5638,7 +5647,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5667,7 +5676,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -5699,7 +5708,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5722,7 +5731,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -5748,7 +5757,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -5771,7 +5780,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -5800,7 +5809,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -5832,7 +5841,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -5858,7 +5867,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A38" s="90" t="s">
+      <c r="A38" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -5887,7 +5896,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -5916,7 +5925,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -5945,7 +5954,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -5974,7 +5983,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -6003,7 +6012,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -6038,7 +6047,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -6064,7 +6073,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -6093,7 +6102,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -6122,7 +6131,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A47" s="90" t="s">
+      <c r="A47" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -6151,7 +6160,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A48" s="90" t="s">
+      <c r="A48" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -6174,7 +6183,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A49" s="90" t="s">
+      <c r="A49" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -6197,7 +6206,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A50" s="90" t="s">
+      <c r="A50" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -6223,7 +6232,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A51" s="90" t="s">
+      <c r="A51" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -6255,7 +6264,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -6281,7 +6290,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A53" s="90" t="s">
+      <c r="A53" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -16426,13 +16435,13 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="90" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.9375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.87890625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.76171875" style="2" customWidth="1"/>
@@ -16450,26 +16459,26 @@
     <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="92" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:15" s="91" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A1" s="90" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="91" t="s">
         <v>1034</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="91" t="s">
         <v>788</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="91" t="s">
         <v>789</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="91" t="s">
         <v>790</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="91" t="s">
         <v>1101</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="91" t="s">
         <v>796</v>
       </c>
       <c r="H1" s="10" t="s">
@@ -16481,16 +16490,16 @@
       <c r="J1" s="10" t="s">
         <v>875</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="91" t="s">
         <v>876</v>
       </c>
-      <c r="L1" s="92" t="s">
+      <c r="L1" s="91" t="s">
         <v>792</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="91" t="s">
         <v>793</v>
       </c>
-      <c r="N1" s="92" t="s">
+      <c r="N1" s="91" t="s">
         <v>794</v>
       </c>
       <c r="O1" s="10" t="s">
@@ -16498,7 +16507,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="30" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B2" s="66" t="s">
@@ -16522,7 +16531,7 @@
       <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B3" s="66" t="s">
@@ -16549,7 +16558,7 @@
       <c r="O3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B4" s="66" t="s">
@@ -16575,7 +16584,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B5" s="66" t="s">
@@ -16603,7 +16612,7 @@
       <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B6" s="66" t="s">
@@ -16631,7 +16640,7 @@
       <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B7" s="66" t="s">
@@ -16661,7 +16670,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B8" s="66" t="s">
@@ -16691,7 +16700,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B9" s="66" t="s">
@@ -16717,7 +16726,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B10" s="66" t="s">
@@ -16745,7 +16754,7 @@
       <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B11" s="66" t="s">
@@ -16773,7 +16782,7 @@
       <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B12" s="66" t="s">
@@ -16801,7 +16810,7 @@
       <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B13" s="66" t="s">
@@ -16831,7 +16840,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B14" s="66" t="s">
@@ -16857,7 +16866,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B15" s="66" t="s">
@@ -16885,7 +16894,7 @@
       <c r="O15" s="16"/>
     </row>
     <row r="16" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B16" s="66" t="s">
@@ -16913,7 +16922,7 @@
       <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B17" s="66" t="s">
@@ -16943,7 +16952,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B18" s="66" t="s">
@@ -16973,7 +16982,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B19" s="66" t="s">
@@ -17010,7 +17019,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B20" s="66" t="s">
@@ -17036,7 +17045,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B21" s="66" t="s">
@@ -17062,7 +17071,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B22" s="66" t="s">
@@ -17091,7 +17100,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B23" s="66" t="s">
@@ -17120,7 +17129,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B24" s="66" t="s">
@@ -17143,7 +17152,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="9" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B25" s="66" t="s">
@@ -17168,7 +17177,7 @@
       <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B26" s="66" t="s">
@@ -17189,7 +17198,9 @@
       <c r="G26" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="16"/>
+      <c r="H26" s="92" t="s">
+        <v>1279</v>
+      </c>
       <c r="I26" s="50" t="s">
         <v>878</v>
       </c>
@@ -17210,7 +17221,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B27" s="66" t="s">
@@ -17236,7 +17247,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B28" s="66" t="s">
@@ -17262,7 +17273,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B29" s="66" t="s">
@@ -17294,7 +17305,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B30" s="66" t="s">
@@ -17323,7 +17334,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" s="9" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B31" s="66" t="s">
@@ -17348,7 +17359,7 @@
       <c r="J31" s="16"/>
     </row>
     <row r="32" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B32" s="66" t="s">
@@ -17383,7 +17394,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B33" s="66" t="s">
@@ -17411,7 +17422,7 @@
       <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B34" s="66" t="s">
@@ -17439,7 +17450,7 @@
       <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B35" s="66" t="s">
@@ -17469,7 +17480,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B36" s="66" t="s">
@@ -17499,7 +17510,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B37" s="66" t="s">
@@ -17534,7 +17545,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="90" t="s">
+      <c r="A38" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B38" s="66" t="s">
@@ -17562,7 +17573,7 @@
       <c r="O38" s="16"/>
     </row>
     <row r="39" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B39" s="66" t="s">
@@ -17590,7 +17601,7 @@
       <c r="O39" s="16"/>
     </row>
     <row r="40" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B40" s="66" t="s">
@@ -17620,7 +17631,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B41" s="66" t="s">
@@ -17650,7 +17661,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B42" s="66" t="s">
@@ -17688,7 +17699,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B43" s="66" t="s">
@@ -17717,7 +17728,7 @@
       <c r="O43" s="16"/>
     </row>
     <row r="44" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B44" s="66" t="s">
@@ -17745,7 +17756,7 @@
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B45" s="66" t="s">
@@ -17775,7 +17786,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B46" s="66" t="s">
@@ -17805,7 +17816,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="90" t="s">
+      <c r="A47" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B47" s="66" t="s">
@@ -17835,7 +17846,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="90" t="s">
+      <c r="A48" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B48" s="66" t="s">
@@ -17864,7 +17875,7 @@
       <c r="O48" s="16"/>
     </row>
     <row r="49" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="90" t="s">
+      <c r="A49" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B49" s="66" t="s">
@@ -17892,7 +17903,7 @@
       <c r="O49" s="16"/>
     </row>
     <row r="50" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="90" t="s">
+      <c r="A50" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B50" s="66" t="s">
@@ -17922,7 +17933,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="90" t="s">
+      <c r="A51" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B51" s="66" t="s">
@@ -17952,7 +17963,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" s="7" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B52" s="66" t="s">
@@ -17979,7 +17990,7 @@
       <c r="O52" s="9"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A53" s="90" t="s">
+      <c r="A53" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B53" s="66" t="s">
@@ -18014,6 +18025,9 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A54" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B54" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18041,7 +18055,9 @@
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="90"/>
+      <c r="A55" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B55" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18070,7 +18086,9 @@
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="90"/>
+      <c r="A56" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B56" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18101,7 +18119,9 @@
       </c>
     </row>
     <row r="57" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="90"/>
+      <c r="A57" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B57" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18132,7 +18152,9 @@
       </c>
     </row>
     <row r="58" spans="1:15" s="7" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A58" s="90"/>
+      <c r="A58" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B58" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18159,7 +18181,9 @@
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="90"/>
+      <c r="A59" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B59" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18196,7 +18220,9 @@
       <c r="O59" s="9"/>
     </row>
     <row r="60" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="90"/>
+      <c r="A60" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B60" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18226,7 +18252,9 @@
       <c r="O60" s="16"/>
     </row>
     <row r="61" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="90"/>
+      <c r="A61" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B61" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18256,7 +18284,9 @@
       <c r="O61" s="16"/>
     </row>
     <row r="62" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="90"/>
+      <c r="A62" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B62" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18288,7 +18318,9 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="90"/>
+      <c r="A63" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B63" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18320,6 +18352,9 @@
       </c>
     </row>
     <row r="64" spans="1:15" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B64" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18355,7 +18390,9 @@
       </c>
     </row>
     <row r="65" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="90"/>
+      <c r="A65" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B65" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18382,7 +18419,9 @@
       <c r="O65" s="16"/>
     </row>
     <row r="66" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="90"/>
+      <c r="A66" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B66" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18408,7 +18447,9 @@
       <c r="O66" s="16"/>
     </row>
     <row r="67" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="90"/>
+      <c r="A67" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B67" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18436,7 +18477,9 @@
       </c>
     </row>
     <row r="68" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A68" s="90"/>
+      <c r="A68" s="89" t="s">
+        <v>1195</v>
+      </c>
       <c r="B68" s="66" t="s">
         <v>1085</v>
       </c>
@@ -18574,13 +18617,13 @@
   <dimension ref="A1:AH90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="90" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.8203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.52734375" customWidth="1"/>
     <col min="4" max="4" width="8.05859375" style="43" customWidth="1"/>
@@ -18626,7 +18669,7 @@
         <v>797</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>798</v>
+        <v>1278</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>799</v>
@@ -18714,7 +18757,7 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B2" s="36" t="s">
@@ -18788,7 +18831,7 @@
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B3" t="s">
@@ -18862,7 +18905,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B4" s="36" t="s">
@@ -18942,7 +18985,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B5" t="s">
@@ -19022,7 +19065,7 @@
       </c>
     </row>
     <row r="6" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B6" s="36" t="s">
@@ -19096,7 +19139,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B7" t="s">
@@ -19170,7 +19213,7 @@
       </c>
     </row>
     <row r="8" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B8" s="36" t="s">
@@ -19235,7 +19278,7 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B9" t="s">
@@ -19294,7 +19337,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B10" s="36" t="s">
@@ -19350,7 +19393,7 @@
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B11" t="s">
@@ -19421,7 +19464,7 @@
       </c>
     </row>
     <row r="12" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B12" s="36" t="s">
@@ -19483,7 +19526,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B13" t="s">
@@ -19557,7 +19600,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B14" s="36" t="s">
@@ -19631,7 +19674,7 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B15" t="s">
@@ -19696,7 +19739,7 @@
       </c>
     </row>
     <row r="16" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B16" s="36" t="s">
@@ -19773,7 +19816,7 @@
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B17" t="s">
@@ -19853,7 +19896,7 @@
       </c>
     </row>
     <row r="18" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B18" s="36" t="s">
@@ -19933,7 +19976,7 @@
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B19" t="s">
@@ -20016,7 +20059,7 @@
       </c>
     </row>
     <row r="20" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B20" s="36" t="s">
@@ -20087,7 +20130,7 @@
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B21" t="s">
@@ -20158,7 +20201,7 @@
       </c>
     </row>
     <row r="22" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B22" s="36" t="s">
@@ -20229,7 +20272,7 @@
       </c>
     </row>
     <row r="23" spans="1:34" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B23" t="s">
@@ -20312,7 +20355,7 @@
       </c>
     </row>
     <row r="24" spans="1:34" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B24" s="36" t="s">
@@ -20374,7 +20417,7 @@
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B25" t="s">
@@ -20433,7 +20476,7 @@
       </c>
     </row>
     <row r="26" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B26" s="36" t="s">
@@ -20510,7 +20553,7 @@
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B27" t="s">
@@ -20587,7 +20630,7 @@
       </c>
     </row>
     <row r="28" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B28" s="36" t="s">
@@ -20667,7 +20710,7 @@
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B29" t="s">
@@ -20750,7 +20793,7 @@
       </c>
     </row>
     <row r="30" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B30" s="36" t="s">
@@ -20821,7 +20864,7 @@
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B31" t="s">
@@ -20892,7 +20935,7 @@
       </c>
     </row>
     <row r="32" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B32" s="36" t="s">
@@ -20963,7 +21006,7 @@
       </c>
     </row>
     <row r="33" spans="1:34" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B33" t="s">
@@ -21046,7 +21089,7 @@
       </c>
     </row>
     <row r="34" spans="1:34" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B34" s="36" t="s">
@@ -21108,7 +21151,7 @@
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B35" t="s">
@@ -21170,7 +21213,7 @@
       </c>
     </row>
     <row r="36" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B36" s="36" t="s">
@@ -21247,7 +21290,7 @@
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B37" t="s">
@@ -21324,7 +21367,7 @@
       </c>
     </row>
     <row r="38" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="90" t="s">
+      <c r="A38" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B38" s="36" t="s">
@@ -21404,7 +21447,7 @@
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B39" t="s">
@@ -21487,7 +21530,7 @@
       </c>
     </row>
     <row r="40" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B40" s="36" t="s">
@@ -21558,7 +21601,7 @@
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B41" t="s">
@@ -21629,7 +21672,7 @@
       </c>
     </row>
     <row r="42" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B42" s="36" t="s">
@@ -21700,7 +21743,7 @@
       </c>
     </row>
     <row r="43" spans="1:34" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B43" t="s">
@@ -21786,7 +21829,7 @@
       </c>
     </row>
     <row r="44" spans="1:34" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B44" s="36" t="s">
@@ -21848,7 +21891,7 @@
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B45" t="s">
@@ -21910,7 +21953,7 @@
       </c>
     </row>
     <row r="46" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B46" s="36" t="s">
@@ -21987,7 +22030,7 @@
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A47" s="90" t="s">
+      <c r="A47" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B47" t="s">
@@ -22064,7 +22107,7 @@
       </c>
     </row>
     <row r="48" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="90" t="s">
+      <c r="A48" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B48" s="36" t="s">
@@ -22144,7 +22187,7 @@
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A49" s="90" t="s">
+      <c r="A49" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B49" t="s">
@@ -22224,7 +22267,7 @@
       </c>
     </row>
     <row r="50" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="90" t="s">
+      <c r="A50" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B50" s="36" t="s">
@@ -22298,7 +22341,7 @@
       </c>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A51" s="90" t="s">
+      <c r="A51" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B51" t="s">
@@ -22372,7 +22415,7 @@
       </c>
     </row>
     <row r="52" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B52" s="36" t="s">
@@ -22437,7 +22480,7 @@
       </c>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A53" s="90" t="s">
+      <c r="A53" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B53" t="s">
@@ -22514,7 +22557,7 @@
       </c>
     </row>
     <row r="54" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="90" t="s">
+      <c r="A54" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B54" s="36" t="s">
@@ -22594,7 +22637,7 @@
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A55" s="90" t="s">
+      <c r="A55" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B55" t="s">
@@ -22683,7 +22726,7 @@
       </c>
     </row>
     <row r="56" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="90" t="s">
+      <c r="A56" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B56" s="36" t="s">
@@ -22760,7 +22803,7 @@
       </c>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A57" s="90" t="s">
+      <c r="A57" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B57" t="s">
@@ -22837,7 +22880,7 @@
       </c>
     </row>
     <row r="58" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="90" t="s">
+      <c r="A58" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B58" s="36" t="s">
@@ -22917,7 +22960,7 @@
       </c>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A59" s="90" t="s">
+      <c r="A59" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B59" t="s">
@@ -22997,7 +23040,7 @@
       </c>
     </row>
     <row r="60" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="90" t="s">
+      <c r="A60" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B60" s="36" t="s">
@@ -23080,7 +23123,7 @@
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A61" s="90" t="s">
+      <c r="A61" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B61" t="s">
@@ -23151,7 +23194,7 @@
       </c>
     </row>
     <row r="62" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B62" s="36" t="s">
@@ -23222,7 +23265,7 @@
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A63" s="90" t="s">
+      <c r="A63" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B63" t="s">
@@ -23293,7 +23336,7 @@
       </c>
     </row>
     <row r="64" spans="1:34" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A64" s="90" t="s">
+      <c r="A64" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B64" s="36" t="s">
@@ -23376,7 +23419,7 @@
       </c>
     </row>
     <row r="65" spans="1:34" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A65" s="90" t="s">
+      <c r="A65" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B65" t="s">
@@ -23435,7 +23478,7 @@
       </c>
     </row>
     <row r="66" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="90" t="s">
+      <c r="A66" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B66" s="36" t="s">
@@ -23494,7 +23537,7 @@
       </c>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A67" s="90" t="s">
+      <c r="A67" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B67" t="s">
@@ -23571,7 +23614,7 @@
       </c>
     </row>
     <row r="68" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A68" s="90" t="s">
+      <c r="A68" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B68" s="36" t="s">
@@ -23648,7 +23691,7 @@
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B69" t="s">
@@ -23731,7 +23774,7 @@
       </c>
     </row>
     <row r="70" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A70" s="90" t="s">
+      <c r="A70" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B70" s="36" t="s">
@@ -23814,7 +23857,7 @@
       </c>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A71" s="90" t="s">
+      <c r="A71" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B71" t="s">
@@ -23888,7 +23931,7 @@
       </c>
     </row>
     <row r="72" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A72" s="90" t="s">
+      <c r="A72" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B72" s="36" t="s">
@@ -23962,7 +24005,7 @@
       </c>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A73" s="90" t="s">
+      <c r="A73" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B73" t="s">
@@ -24027,7 +24070,7 @@
       </c>
     </row>
     <row r="74" spans="1:34" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A74" s="90" t="s">
+      <c r="A74" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B74" s="36" t="s">
@@ -24086,7 +24129,7 @@
       </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A75" s="90" t="s">
+      <c r="A75" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B75" t="s">
@@ -24163,7 +24206,7 @@
       </c>
     </row>
     <row r="76" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A76" s="90" t="s">
+      <c r="A76" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B76" s="36" t="s">
@@ -24243,7 +24286,7 @@
       </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B77" t="s">
@@ -24326,7 +24369,7 @@
       </c>
     </row>
     <row r="78" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="90" t="s">
+      <c r="A78" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B78" s="36" t="s">
@@ -24409,7 +24452,7 @@
       </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.5">
-      <c r="A79" s="90" t="s">
+      <c r="A79" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B79" t="s">
@@ -24483,7 +24526,7 @@
       </c>
     </row>
     <row r="80" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="90" t="s">
+      <c r="A80" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B80" s="36" t="s">
@@ -24557,7 +24600,7 @@
       </c>
     </row>
     <row r="81" spans="1:32" x14ac:dyDescent="0.5">
-      <c r="A81" s="90" t="s">
+      <c r="A81" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B81" t="s">
@@ -24622,7 +24665,7 @@
       </c>
     </row>
     <row r="82" spans="1:32" s="36" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A82" s="90" t="s">
+      <c r="A82" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B82" s="36" t="s">
@@ -24684,7 +24727,7 @@
       </c>
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.5">
-      <c r="A83" s="90" t="s">
+      <c r="A83" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B83" t="s">
@@ -24755,7 +24798,7 @@
       </c>
     </row>
     <row r="84" spans="1:32" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B84" s="36" t="s">
@@ -24829,7 +24872,7 @@
       </c>
     </row>
     <row r="85" spans="1:32" x14ac:dyDescent="0.5">
-      <c r="A85" s="90" t="s">
+      <c r="A85" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B85" t="s">
@@ -24903,7 +24946,7 @@
       </c>
     </row>
     <row r="86" spans="1:32" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A86" s="90" t="s">
+      <c r="A86" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B86" s="36" t="s">
@@ -24980,7 +25023,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" x14ac:dyDescent="0.5">
-      <c r="A87" s="90" t="s">
+      <c r="A87" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B87" t="s">
@@ -25051,7 +25094,7 @@
       </c>
     </row>
     <row r="88" spans="1:32" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A88" s="90" t="s">
+      <c r="A88" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B88" s="36" t="s">
@@ -25122,7 +25165,7 @@
       </c>
     </row>
     <row r="89" spans="1:32" x14ac:dyDescent="0.5">
-      <c r="A89" s="90" t="s">
+      <c r="A89" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B89" t="s">
@@ -25193,7 +25236,7 @@
       </c>
     </row>
     <row r="90" spans="1:32" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A90" s="90"/>
+      <c r="A90" s="89"/>
       <c r="D90" s="55"/>
       <c r="T90" s="49"/>
       <c r="U90" s="49"/>
@@ -25215,14 +25258,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70420D1-4B98-4304-9553-608A7E3461D6}">
   <dimension ref="A1:AG232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D235" sqref="D235"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="90" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.8203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.234375" customWidth="1"/>
     <col min="4" max="4" width="6.9375" style="43" customWidth="1"/>
@@ -25269,7 +25312,7 @@
         <v>797</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>798</v>
+        <v>1278</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>799</v>
@@ -25357,7 +25400,7 @@
       </c>
     </row>
     <row r="2" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -25431,7 +25474,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -25511,7 +25554,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -25588,7 +25631,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -25671,7 +25714,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -25749,7 +25792,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -25827,7 +25870,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -25905,7 +25948,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -25977,7 +26020,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" s="6" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -26051,7 +26094,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -26128,7 +26171,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" s="6" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -26190,7 +26233,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -26268,7 +26311,7 @@
       </c>
     </row>
     <row r="14" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -26349,7 +26392,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -26427,7 +26470,7 @@
       </c>
     </row>
     <row r="16" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B16" s="17" t="s">
@@ -26511,7 +26554,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -26588,7 +26631,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B18" s="17" t="s">
@@ -26662,7 +26705,7 @@
       </c>
     </row>
     <row r="19" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -26736,7 +26779,7 @@
       </c>
     </row>
     <row r="20" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B20" s="17" t="s">
@@ -26804,7 +26847,7 @@
       </c>
     </row>
     <row r="21" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B21" s="17" t="s">
@@ -26878,7 +26921,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B22" s="17" t="s">
@@ -26958,7 +27001,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -27020,7 +27063,7 @@
       </c>
     </row>
     <row r="24" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -27097,7 +27140,7 @@
       </c>
     </row>
     <row r="25" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -27177,7 +27220,7 @@
       </c>
     </row>
     <row r="26" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -27254,7 +27297,7 @@
       </c>
     </row>
     <row r="27" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -27337,7 +27380,7 @@
       </c>
     </row>
     <row r="28" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -27414,7 +27457,7 @@
       </c>
     </row>
     <row r="29" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -27488,7 +27531,7 @@
       </c>
     </row>
     <row r="30" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -27562,7 +27605,7 @@
       </c>
     </row>
     <row r="31" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -27631,7 +27674,7 @@
       </c>
     </row>
     <row r="32" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -27706,7 +27749,7 @@
       </c>
     </row>
     <row r="33" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -27784,7 +27827,7 @@
       </c>
     </row>
     <row r="34" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -27844,7 +27887,7 @@
       </c>
     </row>
     <row r="35" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B35" s="17" t="s">
@@ -27922,7 +27965,7 @@
       </c>
     </row>
     <row r="36" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -28000,7 +28043,7 @@
       </c>
     </row>
     <row r="37" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -28081,7 +28124,7 @@
       </c>
     </row>
     <row r="38" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="90" t="s">
+      <c r="A38" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -28164,7 +28207,7 @@
       </c>
     </row>
     <row r="39" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B39" s="17" t="s">
@@ -28244,7 +28287,7 @@
       </c>
     </row>
     <row r="40" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B40" s="17" t="s">
@@ -28318,7 +28361,7 @@
       </c>
     </row>
     <row r="41" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -28392,7 +28435,7 @@
       </c>
     </row>
     <row r="42" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B42" s="17" t="s">
@@ -28463,7 +28506,7 @@
       </c>
     </row>
     <row r="43" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B43" s="17" t="s">
@@ -28525,7 +28568,7 @@
       </c>
     </row>
     <row r="44" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B44" s="17" t="s">
@@ -28602,7 +28645,7 @@
       </c>
     </row>
     <row r="45" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B45" s="17" t="s">
@@ -28677,7 +28720,7 @@
       </c>
     </row>
     <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -28754,7 +28797,7 @@
       </c>
     </row>
     <row r="47" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="90" t="s">
+      <c r="A47" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -28834,7 +28877,7 @@
       </c>
     </row>
     <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="90" t="s">
+      <c r="A48" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -28911,7 +28954,7 @@
       </c>
     </row>
     <row r="49" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="90" t="s">
+      <c r="A49" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -28994,7 +29037,7 @@
       </c>
     </row>
     <row r="50" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="90" t="s">
+      <c r="A50" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -29072,7 +29115,7 @@
       </c>
     </row>
     <row r="51" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="90" t="s">
+      <c r="A51" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -29147,7 +29190,7 @@
       </c>
     </row>
     <row r="52" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -29222,7 +29265,7 @@
       </c>
     </row>
     <row r="53" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="90" t="s">
+      <c r="A53" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -29291,7 +29334,7 @@
       </c>
     </row>
     <row r="54" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="90" t="s">
+      <c r="A54" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -29366,7 +29409,7 @@
       </c>
     </row>
     <row r="55" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="90" t="s">
+      <c r="A55" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -29443,7 +29486,7 @@
       </c>
     </row>
     <row r="56" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="90" t="s">
+      <c r="A56" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -29502,7 +29545,7 @@
       </c>
     </row>
     <row r="57" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="90" t="s">
+      <c r="A57" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -29580,7 +29623,7 @@
       </c>
     </row>
     <row r="58" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="90" t="s">
+      <c r="A58" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B58" s="17" t="s">
@@ -29661,7 +29704,7 @@
       </c>
     </row>
     <row r="59" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="90" t="s">
+      <c r="A59" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B59" s="17" t="s">
@@ -29739,7 +29782,7 @@
       </c>
     </row>
     <row r="60" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="90" t="s">
+      <c r="A60" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B60" s="17" t="s">
@@ -29823,7 +29866,7 @@
       </c>
     </row>
     <row r="61" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="90" t="s">
+      <c r="A61" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B61" s="17" t="s">
@@ -29901,7 +29944,7 @@
       </c>
     </row>
     <row r="62" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B62" s="17" t="s">
@@ -29976,7 +30019,7 @@
       </c>
     </row>
     <row r="63" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="90" t="s">
+      <c r="A63" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B63" s="17" t="s">
@@ -30051,7 +30094,7 @@
       </c>
     </row>
     <row r="64" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="90" t="s">
+      <c r="A64" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B64" s="17" t="s">
@@ -30120,7 +30163,7 @@
       </c>
     </row>
     <row r="65" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="90" t="s">
+      <c r="A65" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B65" s="17" t="s">
@@ -30195,7 +30238,7 @@
       </c>
     </row>
     <row r="66" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="90" t="s">
+      <c r="A66" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B66" s="17" t="s">
@@ -30273,7 +30316,7 @@
       </c>
     </row>
     <row r="67" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="90" t="s">
+      <c r="A67" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B67" s="17" t="s">
@@ -30333,7 +30376,7 @@
       </c>
     </row>
     <row r="68" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A68" s="90" t="s">
+      <c r="A68" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B68" s="7" t="s">
@@ -30411,7 +30454,7 @@
       </c>
     </row>
     <row r="69" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B69" s="7" t="s">
@@ -30492,7 +30535,7 @@
       </c>
     </row>
     <row r="70" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A70" s="90" t="s">
+      <c r="A70" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -30567,7 +30610,7 @@
       </c>
     </row>
     <row r="71" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A71" s="90" t="s">
+      <c r="A71" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B71" s="7" t="s">
@@ -30645,7 +30688,7 @@
       </c>
     </row>
     <row r="72" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A72" s="90" t="s">
+      <c r="A72" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B72" s="7" t="s">
@@ -30720,7 +30763,7 @@
       </c>
     </row>
     <row r="73" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A73" s="90" t="s">
+      <c r="A73" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B73" s="7" t="s">
@@ -30792,7 +30835,7 @@
       </c>
     </row>
     <row r="74" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A74" s="90" t="s">
+      <c r="A74" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -30864,7 +30907,7 @@
       </c>
     </row>
     <row r="75" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="90" t="s">
+      <c r="A75" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B75" s="7" t="s">
@@ -30933,7 +30976,7 @@
       </c>
     </row>
     <row r="76" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A76" s="90" t="s">
+      <c r="A76" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B76" s="7" t="s">
@@ -31005,7 +31048,7 @@
       </c>
     </row>
     <row r="77" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -31080,7 +31123,7 @@
       </c>
     </row>
     <row r="78" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="90" t="s">
+      <c r="A78" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -31140,7 +31183,7 @@
       </c>
     </row>
     <row r="79" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A79" s="90" t="s">
+      <c r="A79" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B79" s="26" t="s">
@@ -31218,7 +31261,7 @@
       </c>
     </row>
     <row r="80" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="90" t="s">
+      <c r="A80" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B80" s="26" t="s">
@@ -31299,7 +31342,7 @@
       </c>
     </row>
     <row r="81" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A81" s="90" t="s">
+      <c r="A81" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B81" s="26" t="s">
@@ -31374,7 +31417,7 @@
       </c>
     </row>
     <row r="82" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A82" s="90" t="s">
+      <c r="A82" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B82" s="26" t="s">
@@ -31452,7 +31495,7 @@
       </c>
     </row>
     <row r="83" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A83" s="90" t="s">
+      <c r="A83" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B83" s="26" t="s">
@@ -31527,7 +31570,7 @@
       </c>
     </row>
     <row r="84" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A84" s="90" t="s">
+      <c r="A84" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B84" s="26" t="s">
@@ -31599,7 +31642,7 @@
       </c>
     </row>
     <row r="85" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A85" s="90" t="s">
+      <c r="A85" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B85" s="26" t="s">
@@ -31671,7 +31714,7 @@
       </c>
     </row>
     <row r="86" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A86" s="90" t="s">
+      <c r="A86" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B86" s="26" t="s">
@@ -31740,7 +31783,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A87" s="90" t="s">
+      <c r="A87" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B87" s="26" t="s">
@@ -31812,7 +31855,7 @@
       </c>
     </row>
     <row r="88" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A88" s="90" t="s">
+      <c r="A88" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B88" s="26" t="s">
@@ -31887,7 +31930,7 @@
       </c>
     </row>
     <row r="89" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A89" s="90" t="s">
+      <c r="A89" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B89" s="26" t="s">
@@ -31947,7 +31990,7 @@
       </c>
     </row>
     <row r="90" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A90" s="90" t="s">
+      <c r="A90" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B90" s="26" t="s">
@@ -32004,7 +32047,7 @@
       </c>
     </row>
     <row r="91" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A91" s="90" t="s">
+      <c r="A91" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B91" s="6" t="s">
@@ -32070,7 +32113,7 @@
       </c>
     </row>
     <row r="92" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A92" s="90" t="s">
+      <c r="A92" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B92" s="6" t="s">
@@ -32133,7 +32176,7 @@
       </c>
     </row>
     <row r="93" spans="1:32" s="6" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A93" s="90" t="s">
+      <c r="A93" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B93" s="6" t="s">
@@ -32190,7 +32233,7 @@
       </c>
     </row>
     <row r="94" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A94" s="90" t="s">
+      <c r="A94" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B94" s="6" t="s">
@@ -32262,7 +32305,7 @@
       </c>
     </row>
     <row r="95" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A95" s="90" t="s">
+      <c r="A95" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B95" s="6" t="s">
@@ -32334,7 +32377,7 @@
       </c>
     </row>
     <row r="96" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A96" s="90" t="s">
+      <c r="A96" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B96" s="6" t="s">
@@ -32391,7 +32434,7 @@
       </c>
     </row>
     <row r="97" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A97" s="90" t="s">
+      <c r="A97" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B97" s="6" t="s">
@@ -32454,7 +32497,7 @@
       </c>
     </row>
     <row r="98" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A98" s="90" t="s">
+      <c r="A98" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B98" s="6" t="s">
@@ -32514,7 +32557,7 @@
       </c>
     </row>
     <row r="99" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A99" s="90" t="s">
+      <c r="A99" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B99" s="6" t="s">
@@ -32571,7 +32614,7 @@
       </c>
     </row>
     <row r="100" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A100" s="90" t="s">
+      <c r="A100" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B100" s="17" t="s">
@@ -32634,7 +32677,7 @@
       </c>
     </row>
     <row r="101" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A101" s="90" t="s">
+      <c r="A101" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -32715,7 +32758,7 @@
       </c>
     </row>
     <row r="102" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A102" s="90" t="s">
+      <c r="A102" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B102" s="17" t="s">
@@ -32793,7 +32836,7 @@
       </c>
     </row>
     <row r="103" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A103" s="90" t="s">
+      <c r="A103" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B103" s="17" t="s">
@@ -32877,7 +32920,7 @@
       </c>
     </row>
     <row r="104" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A104" s="90" t="s">
+      <c r="A104" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B104" s="17" t="s">
@@ -32955,7 +32998,7 @@
       </c>
     </row>
     <row r="105" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A105" s="90" t="s">
+      <c r="A105" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B105" s="17" t="s">
@@ -33033,7 +33076,7 @@
       </c>
     </row>
     <row r="106" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A106" s="90" t="s">
+      <c r="A106" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B106" s="17" t="s">
@@ -33111,7 +33154,7 @@
       </c>
     </row>
     <row r="107" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A107" s="90" t="s">
+      <c r="A107" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B107" s="17" t="s">
@@ -33183,7 +33226,7 @@
       </c>
     </row>
     <row r="108" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A108" s="90" t="s">
+      <c r="A108" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B108" s="17" t="s">
@@ -33258,7 +33301,7 @@
       </c>
     </row>
     <row r="109" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A109" s="90" t="s">
+      <c r="A109" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B109" s="17" t="s">
@@ -33336,7 +33379,7 @@
       </c>
     </row>
     <row r="110" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A110" s="90" t="s">
+      <c r="A110" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B110" s="17" t="s">
@@ -33396,7 +33439,7 @@
       </c>
     </row>
     <row r="111" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A111" s="90" t="s">
+      <c r="A111" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B111" s="6" t="s">
@@ -33474,7 +33517,7 @@
       </c>
     </row>
     <row r="112" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A112" s="90" t="s">
+      <c r="A112" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B112" s="6" t="s">
@@ -33555,7 +33598,7 @@
       </c>
     </row>
     <row r="113" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A113" s="90" t="s">
+      <c r="A113" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B113" s="6" t="s">
@@ -33633,7 +33676,7 @@
       </c>
     </row>
     <row r="114" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A114" s="90" t="s">
+      <c r="A114" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B114" s="6" t="s">
@@ -33717,7 +33760,7 @@
       </c>
     </row>
     <row r="115" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A115" s="90" t="s">
+      <c r="A115" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B115" s="6" t="s">
@@ -33795,7 +33838,7 @@
       </c>
     </row>
     <row r="116" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A116" s="90" t="s">
+      <c r="A116" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B116" s="6" t="s">
@@ -33873,7 +33916,7 @@
       </c>
     </row>
     <row r="117" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A117" s="90" t="s">
+      <c r="A117" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B117" s="6" t="s">
@@ -33951,7 +33994,7 @@
       </c>
     </row>
     <row r="118" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A118" s="90" t="s">
+      <c r="A118" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -34023,7 +34066,7 @@
       </c>
     </row>
     <row r="119" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A119" s="90" t="s">
+      <c r="A119" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B119" s="6" t="s">
@@ -34098,7 +34141,7 @@
       </c>
     </row>
     <row r="120" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A120" s="90" t="s">
+      <c r="A120" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B120" s="6" t="s">
@@ -34176,7 +34219,7 @@
       </c>
     </row>
     <row r="121" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A121" s="90" t="s">
+      <c r="A121" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B121" s="6" t="s">
@@ -34236,7 +34279,7 @@
       </c>
     </row>
     <row r="122" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A122" s="90" t="s">
+      <c r="A122" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B122" s="17" t="s">
@@ -34311,7 +34354,7 @@
       </c>
     </row>
     <row r="123" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A123" s="90" t="s">
+      <c r="A123" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B123" s="17" t="s">
@@ -34389,7 +34432,7 @@
       </c>
     </row>
     <row r="124" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A124" s="90" t="s">
+      <c r="A124" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B124" s="17" t="s">
@@ -34467,7 +34510,7 @@
       </c>
     </row>
     <row r="125" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A125" s="90" t="s">
+      <c r="A125" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B125" s="17" t="s">
@@ -34551,7 +34594,7 @@
       </c>
     </row>
     <row r="126" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A126" s="90" t="s">
+      <c r="A126" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B126" s="17" t="s">
@@ -34629,7 +34672,7 @@
       </c>
     </row>
     <row r="127" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A127" s="90" t="s">
+      <c r="A127" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B127" s="17" t="s">
@@ -34695,7 +34738,7 @@
       </c>
     </row>
     <row r="128" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A128" s="90" t="s">
+      <c r="A128" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B128" s="17" t="s">
@@ -34761,7 +34804,7 @@
       </c>
     </row>
     <row r="129" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A129" s="90" t="s">
+      <c r="A129" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B129" s="17" t="s">
@@ -34833,7 +34876,7 @@
       </c>
     </row>
     <row r="130" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A130" s="90" t="s">
+      <c r="A130" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B130" s="17" t="s">
@@ -34911,7 +34954,7 @@
       </c>
     </row>
     <row r="131" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A131" s="90" t="s">
+      <c r="A131" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B131" s="17" t="s">
@@ -34989,7 +35032,7 @@
       </c>
     </row>
     <row r="132" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A132" s="90" t="s">
+      <c r="A132" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B132" s="17" t="s">
@@ -35052,7 +35095,7 @@
       </c>
     </row>
     <row r="133" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A133" s="90" t="s">
+      <c r="A133" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B133" s="17" t="s">
@@ -35112,7 +35155,7 @@
       </c>
     </row>
     <row r="134" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A134" s="90" t="s">
+      <c r="A134" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B134" s="6" t="s">
@@ -35190,7 +35233,7 @@
       </c>
     </row>
     <row r="135" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A135" s="90" t="s">
+      <c r="A135" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B135" s="6" t="s">
@@ -35265,7 +35308,7 @@
       </c>
     </row>
     <row r="136" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A136" s="90" t="s">
+      <c r="A136" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B136" s="6" t="s">
@@ -35346,7 +35389,7 @@
       </c>
     </row>
     <row r="137" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A137" s="90" t="s">
+      <c r="A137" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B137" s="6" t="s">
@@ -35424,7 +35467,7 @@
       </c>
     </row>
     <row r="138" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A138" s="90" t="s">
+      <c r="A138" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B138" s="6" t="s">
@@ -35511,7 +35554,7 @@
       </c>
     </row>
     <row r="139" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A139" s="90" t="s">
+      <c r="A139" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B139" s="6" t="s">
@@ -35583,7 +35626,7 @@
       </c>
     </row>
     <row r="140" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A140" s="90" t="s">
+      <c r="A140" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B140" s="6" t="s">
@@ -35661,7 +35704,7 @@
       </c>
     </row>
     <row r="141" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A141" s="90" t="s">
+      <c r="A141" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B141" s="6" t="s">
@@ -35748,7 +35791,7 @@
       </c>
     </row>
     <row r="142" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A142" s="90" t="s">
+      <c r="A142" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B142" s="6" t="s">
@@ -35811,7 +35854,7 @@
       </c>
     </row>
     <row r="143" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A143" s="90" t="s">
+      <c r="A143" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B143" s="6" t="s">
@@ -35889,7 +35932,7 @@
       </c>
     </row>
     <row r="144" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A144" s="90" t="s">
+      <c r="A144" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B144" s="6" t="s">
@@ -35958,7 +36001,7 @@
       </c>
     </row>
     <row r="145" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A145" s="90" t="s">
+      <c r="A145" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B145" s="17" t="s">
@@ -36036,7 +36079,7 @@
       </c>
     </row>
     <row r="146" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A146" s="90" t="s">
+      <c r="A146" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B146" s="17" t="s">
@@ -36117,7 +36160,7 @@
       </c>
     </row>
     <row r="147" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A147" s="90" t="s">
+      <c r="A147" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B147" s="17" t="s">
@@ -36195,7 +36238,7 @@
       </c>
     </row>
     <row r="148" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A148" s="90" t="s">
+      <c r="A148" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B148" s="17" t="s">
@@ -36279,7 +36322,7 @@
       </c>
     </row>
     <row r="149" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A149" s="90" t="s">
+      <c r="A149" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B149" s="17" t="s">
@@ -36357,7 +36400,7 @@
       </c>
     </row>
     <row r="150" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A150" s="90" t="s">
+      <c r="A150" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B150" s="17" t="s">
@@ -36432,7 +36475,7 @@
       </c>
     </row>
     <row r="151" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A151" s="90" t="s">
+      <c r="A151" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B151" s="17" t="s">
@@ -36507,7 +36550,7 @@
       </c>
     </row>
     <row r="152" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A152" s="90" t="s">
+      <c r="A152" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B152" s="17" t="s">
@@ -36576,7 +36619,7 @@
       </c>
     </row>
     <row r="153" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A153" s="90" t="s">
+      <c r="A153" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B153" s="17" t="s">
@@ -36651,7 +36694,7 @@
       </c>
     </row>
     <row r="154" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A154" s="90" t="s">
+      <c r="A154" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B154" s="17" t="s">
@@ -36729,7 +36772,7 @@
       </c>
     </row>
     <row r="155" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A155" s="90" t="s">
+      <c r="A155" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B155" s="17" t="s">
@@ -36789,7 +36832,7 @@
       </c>
     </row>
     <row r="156" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A156" s="90" t="s">
+      <c r="A156" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B156" s="6" t="s">
@@ -36867,7 +36910,7 @@
       </c>
     </row>
     <row r="157" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A157" s="90" t="s">
+      <c r="A157" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B157" s="6" t="s">
@@ -36948,7 +36991,7 @@
       </c>
     </row>
     <row r="158" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A158" s="90" t="s">
+      <c r="A158" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B158" s="6" t="s">
@@ -37026,7 +37069,7 @@
       </c>
     </row>
     <row r="159" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A159" s="90" t="s">
+      <c r="A159" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B159" s="6" t="s">
@@ -37110,7 +37153,7 @@
       </c>
     </row>
     <row r="160" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A160" s="90" t="s">
+      <c r="A160" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B160" s="6" t="s">
@@ -37188,7 +37231,7 @@
       </c>
     </row>
     <row r="161" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A161" s="90" t="s">
+      <c r="A161" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B161" s="6" t="s">
@@ -37263,7 +37306,7 @@
       </c>
     </row>
     <row r="162" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A162" s="90" t="s">
+      <c r="A162" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B162" s="6" t="s">
@@ -37338,7 +37381,7 @@
       </c>
     </row>
     <row r="163" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A163" s="90" t="s">
+      <c r="A163" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B163" s="6" t="s">
@@ -37407,7 +37450,7 @@
       </c>
     </row>
     <row r="164" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A164" s="90" t="s">
+      <c r="A164" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B164" s="6" t="s">
@@ -37482,7 +37525,7 @@
       </c>
     </row>
     <row r="165" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A165" s="90" t="s">
+      <c r="A165" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B165" s="6" t="s">
@@ -37560,7 +37603,7 @@
       </c>
     </row>
     <row r="166" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A166" s="90" t="s">
+      <c r="A166" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B166" s="6" t="s">
@@ -37620,7 +37663,7 @@
       </c>
     </row>
     <row r="167" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A167" s="90" t="s">
+      <c r="A167" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B167" s="17" t="s">
@@ -37698,7 +37741,7 @@
       </c>
     </row>
     <row r="168" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A168" s="90" t="s">
+      <c r="A168" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B168" s="17" t="s">
@@ -37779,7 +37822,7 @@
       </c>
     </row>
     <row r="169" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A169" s="90" t="s">
+      <c r="A169" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B169" s="17" t="s">
@@ -37857,7 +37900,7 @@
       </c>
     </row>
     <row r="170" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A170" s="90" t="s">
+      <c r="A170" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B170" s="17" t="s">
@@ -37941,7 +37984,7 @@
       </c>
     </row>
     <row r="171" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A171" s="90" t="s">
+      <c r="A171" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B171" s="17" t="s">
@@ -38019,7 +38062,7 @@
       </c>
     </row>
     <row r="172" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A172" s="90" t="s">
+      <c r="A172" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B172" s="17" t="s">
@@ -38097,7 +38140,7 @@
       </c>
     </row>
     <row r="173" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A173" s="90" t="s">
+      <c r="A173" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B173" s="17" t="s">
@@ -38175,7 +38218,7 @@
       </c>
     </row>
     <row r="174" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A174" s="90" t="s">
+      <c r="A174" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B174" s="17" t="s">
@@ -38247,7 +38290,7 @@
       </c>
     </row>
     <row r="175" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A175" s="90" t="s">
+      <c r="A175" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B175" s="17" t="s">
@@ -38322,7 +38365,7 @@
       </c>
     </row>
     <row r="176" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A176" s="90" t="s">
+      <c r="A176" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B176" s="17" t="s">
@@ -38400,7 +38443,7 @@
       </c>
     </row>
     <row r="177" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A177" s="90" t="s">
+      <c r="A177" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B177" s="17" t="s">
@@ -38460,7 +38503,7 @@
       </c>
     </row>
     <row r="178" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A178" s="90" t="s">
+      <c r="A178" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B178" s="6" t="s">
@@ -38539,7 +38582,7 @@
       </c>
     </row>
     <row r="179" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A179" s="90" t="s">
+      <c r="A179" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B179" s="6" t="s">
@@ -38620,7 +38663,7 @@
       </c>
     </row>
     <row r="180" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A180" s="90" t="s">
+      <c r="A180" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B180" s="6" t="s">
@@ -38698,7 +38741,7 @@
       </c>
     </row>
     <row r="181" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A181" s="90" t="s">
+      <c r="A181" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B181" s="6" t="s">
@@ -38782,7 +38825,7 @@
       </c>
     </row>
     <row r="182" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A182" s="90" t="s">
+      <c r="A182" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B182" s="6" t="s">
@@ -38860,7 +38903,7 @@
       </c>
     </row>
     <row r="183" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A183" s="90" t="s">
+      <c r="A183" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B183" s="6" t="s">
@@ -38938,7 +38981,7 @@
       </c>
     </row>
     <row r="184" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A184" s="90" t="s">
+      <c r="A184" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B184" s="6" t="s">
@@ -39016,7 +39059,7 @@
       </c>
     </row>
     <row r="185" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A185" s="90" t="s">
+      <c r="A185" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B185" s="6" t="s">
@@ -39088,7 +39131,7 @@
       </c>
     </row>
     <row r="186" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A186" s="90" t="s">
+      <c r="A186" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B186" s="6" t="s">
@@ -39163,7 +39206,7 @@
       </c>
     </row>
     <row r="187" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A187" s="90" t="s">
+      <c r="A187" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B187" s="6" t="s">
@@ -39241,7 +39284,7 @@
       </c>
     </row>
     <row r="188" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A188" s="90" t="s">
+      <c r="A188" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B188" s="6" t="s">
@@ -39301,7 +39344,7 @@
       </c>
     </row>
     <row r="189" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A189" s="90" t="s">
+      <c r="A189" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B189" s="17" t="s">
@@ -39379,7 +39422,7 @@
       </c>
     </row>
     <row r="190" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A190" s="90" t="s">
+      <c r="A190" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B190" s="17" t="s">
@@ -39460,7 +39503,7 @@
       </c>
     </row>
     <row r="191" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A191" s="90" t="s">
+      <c r="A191" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B191" s="17" t="s">
@@ -39538,7 +39581,7 @@
       </c>
     </row>
     <row r="192" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A192" s="90" t="s">
+      <c r="A192" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B192" s="17" t="s">
@@ -39622,7 +39665,7 @@
       </c>
     </row>
     <row r="193" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A193" s="90" t="s">
+      <c r="A193" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B193" s="17" t="s">
@@ -39700,7 +39743,7 @@
       </c>
     </row>
     <row r="194" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A194" s="90" t="s">
+      <c r="A194" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B194" s="17" t="s">
@@ -39778,7 +39821,7 @@
       </c>
     </row>
     <row r="195" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A195" s="90" t="s">
+      <c r="A195" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B195" s="17" t="s">
@@ -39856,7 +39899,7 @@
       </c>
     </row>
     <row r="196" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A196" s="90" t="s">
+      <c r="A196" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B196" s="17" t="s">
@@ -39928,7 +39971,7 @@
       </c>
     </row>
     <row r="197" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A197" s="90" t="s">
+      <c r="A197" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B197" s="17" t="s">
@@ -40003,7 +40046,7 @@
       </c>
     </row>
     <row r="198" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A198" s="90" t="s">
+      <c r="A198" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B198" s="17" t="s">
@@ -40081,7 +40124,7 @@
       </c>
     </row>
     <row r="199" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A199" s="90" t="s">
+      <c r="A199" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B199" s="17" t="s">
@@ -40141,7 +40184,7 @@
       </c>
     </row>
     <row r="200" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A200" s="90" t="s">
+      <c r="A200" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B200" s="6" t="s">
@@ -40219,7 +40262,7 @@
       </c>
     </row>
     <row r="201" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A201" s="90" t="s">
+      <c r="A201" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B201" s="6" t="s">
@@ -40300,7 +40343,7 @@
       </c>
     </row>
     <row r="202" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A202" s="90" t="s">
+      <c r="A202" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B202" s="6" t="s">
@@ -40378,7 +40421,7 @@
       </c>
     </row>
     <row r="203" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A203" s="90" t="s">
+      <c r="A203" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B203" s="6" t="s">
@@ -40462,7 +40505,7 @@
       </c>
     </row>
     <row r="204" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A204" s="90" t="s">
+      <c r="A204" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B204" s="6" t="s">
@@ -40540,7 +40583,7 @@
       </c>
     </row>
     <row r="205" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A205" s="90" t="s">
+      <c r="A205" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B205" s="6" t="s">
@@ -40618,7 +40661,7 @@
       </c>
     </row>
     <row r="206" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A206" s="90" t="s">
+      <c r="A206" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B206" s="6" t="s">
@@ -40696,7 +40739,7 @@
       </c>
     </row>
     <row r="207" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A207" s="90" t="s">
+      <c r="A207" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B207" s="6" t="s">
@@ -40768,7 +40811,7 @@
       </c>
     </row>
     <row r="208" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A208" s="90" t="s">
+      <c r="A208" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B208" s="6" t="s">
@@ -40840,7 +40883,7 @@
       </c>
     </row>
     <row r="209" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A209" s="90" t="s">
+      <c r="A209" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B209" s="6" t="s">
@@ -40918,7 +40961,7 @@
       </c>
     </row>
     <row r="210" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A210" s="90" t="s">
+      <c r="A210" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B210" s="6" t="s">
@@ -40978,7 +41021,7 @@
       </c>
     </row>
     <row r="211" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A211" s="90" t="s">
+      <c r="A211" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B211" s="17" t="s">
@@ -41056,7 +41099,7 @@
       </c>
     </row>
     <row r="212" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A212" s="90" t="s">
+      <c r="A212" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B212" s="17" t="s">
@@ -41137,7 +41180,7 @@
       </c>
     </row>
     <row r="213" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A213" s="90" t="s">
+      <c r="A213" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B213" s="17" t="s">
@@ -41215,7 +41258,7 @@
       </c>
     </row>
     <row r="214" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A214" s="90" t="s">
+      <c r="A214" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B214" s="17" t="s">
@@ -41299,7 +41342,7 @@
       </c>
     </row>
     <row r="215" spans="1:33" s="17" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A215" s="90" t="s">
+      <c r="A215" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B215" s="17" t="s">
@@ -41377,7 +41420,7 @@
       </c>
     </row>
     <row r="216" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A216" s="90" t="s">
+      <c r="A216" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B216" s="17" t="s">
@@ -41455,7 +41498,7 @@
       </c>
     </row>
     <row r="217" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A217" s="90" t="s">
+      <c r="A217" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B217" s="17" t="s">
@@ -41533,7 +41576,7 @@
       </c>
     </row>
     <row r="218" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A218" s="90" t="s">
+      <c r="A218" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B218" s="17" t="s">
@@ -41605,7 +41648,7 @@
       </c>
     </row>
     <row r="219" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A219" s="90" t="s">
+      <c r="A219" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B219" s="17" t="s">
@@ -41680,7 +41723,7 @@
       </c>
     </row>
     <row r="220" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A220" s="90" t="s">
+      <c r="A220" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B220" s="17" t="s">
@@ -41758,7 +41801,7 @@
       </c>
     </row>
     <row r="221" spans="1:33" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A221" s="90" t="s">
+      <c r="A221" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B221" s="17" t="s">
@@ -41818,7 +41861,7 @@
       </c>
     </row>
     <row r="222" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A222" s="90" t="s">
+      <c r="A222" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B222" s="6" t="s">
@@ -41896,7 +41939,7 @@
       </c>
     </row>
     <row r="223" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A223" s="90" t="s">
+      <c r="A223" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B223" s="6" t="s">
@@ -41977,7 +42020,7 @@
       </c>
     </row>
     <row r="224" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A224" s="90" t="s">
+      <c r="A224" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B224" s="6" t="s">
@@ -42055,7 +42098,7 @@
       </c>
     </row>
     <row r="225" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A225" s="90" t="s">
+      <c r="A225" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B225" s="6" t="s">
@@ -42139,7 +42182,7 @@
       </c>
     </row>
     <row r="226" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A226" s="90" t="s">
+      <c r="A226" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B226" s="6" t="s">
@@ -42217,7 +42260,7 @@
       </c>
     </row>
     <row r="227" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A227" s="90" t="s">
+      <c r="A227" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -42295,7 +42338,7 @@
       </c>
     </row>
     <row r="228" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A228" s="90" t="s">
+      <c r="A228" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B228" s="6" t="s">
@@ -42373,7 +42416,7 @@
       </c>
     </row>
     <row r="229" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A229" s="90" t="s">
+      <c r="A229" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B229" s="6" t="s">
@@ -42445,7 +42488,7 @@
       </c>
     </row>
     <row r="230" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A230" s="90" t="s">
+      <c r="A230" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B230" s="6" t="s">
@@ -42520,7 +42563,7 @@
       </c>
     </row>
     <row r="231" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A231" s="90" t="s">
+      <c r="A231" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B231" s="6" t="s">
@@ -42598,7 +42641,7 @@
       </c>
     </row>
     <row r="232" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A232" s="90" t="s">
+      <c r="A232" s="89" t="s">
         <v>1195</v>
       </c>
       <c r="B232" s="6" t="s">
@@ -49752,10 +49795,10 @@
       <c r="F28" s="70" t="s">
         <v>1069</v>
       </c>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
       <c r="K28" s="69"/>
       <c r="L28" s="69"/>
       <c r="M28" s="69"/>
@@ -49774,8 +49817,8 @@
       </c>
       <c r="E29" s="69"/>
       <c r="F29" s="70"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="93"/>
       <c r="I29" s="69"/>
       <c r="J29" s="47" t="s">
         <v>857</v>
@@ -49802,8 +49845,8 @@
       </c>
       <c r="E30" s="69"/>
       <c r="F30" s="70"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="93"/>
       <c r="I30" s="69"/>
       <c r="J30" s="47" t="s">
         <v>995</v>
@@ -49832,8 +49875,8 @@
       </c>
       <c r="E31" s="69"/>
       <c r="F31" s="70"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="89"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
       <c r="I31" s="69"/>
       <c r="J31" s="47" t="s">
         <v>998</v>
@@ -49860,8 +49903,8 @@
       </c>
       <c r="E32" s="69"/>
       <c r="F32" s="70"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="93"/>
       <c r="I32" s="69"/>
       <c r="J32" s="47" t="s">
         <v>1000</v>
@@ -50190,13 +50233,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A74BE6FB-E381-48E9-AFEA-0E3F4988ACEE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3E06F1B-2DC0-499B-831C-0AF867B66031}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEB72D98-24B2-438A-8EBB-0825914E34A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AFDF3A5-2895-433F-8B05-7DDEB0AEB8C3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7401B04-B25C-4D32-ADB7-897552C61E69}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59F9E161-C85A-46D0-A8DD-56AF016D0B1A}"/>
 </file>
</xml_diff>

<commit_message>
Update SDTM YAML - add valuelists for subset codelists
</commit_message>
<xml_diff>
--- a/BC Curation Template.xlsx
+++ b/BC Curation Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48804EC8-0D87-454B-9E63-EF8A88462A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C867DE-32D9-4D35-874A-E0D84E6D4EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="2" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
@@ -18362,7 +18362,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N50" sqref="N50"/>
+      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21958,10 +21958,10 @@
         <v>104</v>
       </c>
       <c r="L49" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="M49" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="N49" t="s">
         <v>729</v>
@@ -49959,20 +49959,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49995,14 +49995,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AFDF3A5-2895-433F-8B05-7DDEB0AEB8C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59F9E161-C85A-46D0-A8DD-56AF016D0B1A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -50010,4 +50002,12 @@
     <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AFDF3A5-2895-433F-8B05-7DDEB0AEB8C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>